<commit_message>
mostrando viabilidad - final de prueba inicial
</commit_message>
<xml_diff>
--- a/archivo - copia.xlsx
+++ b/archivo - copia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio\github\cripto_fores_trading\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F159C715-EC7A-4284-9962-12858B4D0D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618B2DCD-99A1-479D-8B4C-AC2B5C65BD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>ven0</t>
   </si>
@@ -86,13 +86,16 @@
   </si>
   <si>
     <t>volv3</t>
+  </si>
+  <si>
+    <t>prueba</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +105,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -155,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -163,6 +174,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,9 +513,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -578,6 +592,19 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>